<commit_message>
First cut (not tested) of three-factor storage Excel function.
</commit_message>
<xml_diff>
--- a/samples/excel/three_factor_storage.xlsx
+++ b/samples/excel/three_factor_storage.xlsx
@@ -8,13 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jake\source\repos\storage\samples\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6940367E-8BF6-42DC-95A1-0781EEAE6275}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88BB0B0E-9F51-474C-B74D-77D1ACAF5A6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="585" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Storage" sheetId="1" r:id="rId1"/>
+    <sheet name="Monte Carlo Parameters" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="McParams.BasisFuncs">'Monte Carlo Parameters'!$C$8</definedName>
+    <definedName name="McParams.ExtraDecs">'Monte Carlo Parameters'!$C$7</definedName>
+    <definedName name="McParams.FwdSeed">'Monte Carlo Parameters'!$C$4</definedName>
+    <definedName name="McParams.GridPoints">'Monte Carlo Parameters'!$C$5</definedName>
+    <definedName name="McParams.NumSims">'Monte Carlo Parameters'!$C$2</definedName>
+    <definedName name="McParams.NumTol">'Monte Carlo Parameters'!$C$6</definedName>
+    <definedName name="McParams.Seed">'Monte Carlo Parameters'!$C$3</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -55,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>Inject/Withdraw/Inventory Constraints</t>
   </si>
@@ -97,6 +107,57 @@
   </si>
   <si>
     <t>storage1</t>
+  </si>
+  <si>
+    <t>Num Sim</t>
+  </si>
+  <si>
+    <t>Seed</t>
+  </si>
+  <si>
+    <t>Fwd Seed</t>
+  </si>
+  <si>
+    <t>Grid Points</t>
+  </si>
+  <si>
+    <t>Numerical Tolerance</t>
+  </si>
+  <si>
+    <t>Basis Functions</t>
+  </si>
+  <si>
+    <t>Extra Decisions</t>
+  </si>
+  <si>
+    <t>1 + x_st + x_sw + x_lt + x_st**2 + x_sw**2 + x_lt**2 + x_st**3 + x_sw**3 + x_lt**3</t>
+  </si>
+  <si>
+    <t>Valuation Date</t>
+  </si>
+  <si>
+    <t>2-Factor Parameters</t>
+  </si>
+  <si>
+    <t>Spot Vol</t>
+  </si>
+  <si>
+    <t>Spot Mean Reversion</t>
+  </si>
+  <si>
+    <t>Long Term Vol</t>
+  </si>
+  <si>
+    <t>Seasonal Vol</t>
+  </si>
+  <si>
+    <t>Discount Deltas</t>
+  </si>
+  <si>
+    <t>Piecewise Flat Forward Curve</t>
+  </si>
+  <si>
+    <t>Price</t>
   </si>
 </sst>
 </file>
@@ -184,7 +245,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -198,6 +259,7 @@
     <xf numFmtId="4" fontId="1" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -480,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:H291"/>
+  <dimension ref="B2:N291"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,9 +553,12 @@
     <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
@@ -505,7 +570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
@@ -513,7 +578,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M4" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="E5" s="1" t="s">
         <v>3</v>
       </c>
@@ -526,8 +596,14 @@
       <c r="H5" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="M5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
@@ -546,8 +622,20 @@
       <c r="H6" s="4">
         <v>305</v>
       </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" s="3">
+        <v>43581</v>
+      </c>
+      <c r="M6" s="3">
+        <v>43702</v>
+      </c>
+      <c r="N6" s="13">
+        <v>50.640695748227039</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
@@ -566,8 +654,20 @@
       <c r="H7" s="4">
         <v>337.8</v>
       </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0</v>
+      </c>
+      <c r="M7" s="3">
+        <v>43703</v>
+      </c>
+      <c r="N7" s="13">
+        <v>49.700092287036142</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="E8" s="3">
         <v>43556</v>
       </c>
@@ -580,8 +680,20 @@
       <c r="H8" s="4">
         <v>342.2</v>
       </c>
-    </row>
-    <row r="9" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K8" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M8" s="3">
+        <v>43709</v>
+      </c>
+      <c r="N8" s="13">
+        <v>52.68</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
@@ -597,8 +709,14 @@
       <c r="H9" s="4">
         <v>356.8</v>
       </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="M9" s="3">
+        <v>43739</v>
+      </c>
+      <c r="N9" s="13">
+        <v>55.87</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
@@ -617,8 +735,17 @@
       <c r="H10" s="6">
         <v>295.85000000000002</v>
       </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M10" s="3">
+        <v>43770</v>
+      </c>
+      <c r="N10" s="13">
+        <v>57.89</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
@@ -637,8 +764,20 @@
       <c r="H11" s="8">
         <v>327.666</v>
       </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K11" s="2">
+        <v>0.51</v>
+      </c>
+      <c r="M11" s="3">
+        <v>43800</v>
+      </c>
+      <c r="N11" s="13">
+        <v>59.48</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="E12" s="7">
         <v>43709</v>
       </c>
@@ -651,8 +790,20 @@
       <c r="H12" s="8">
         <v>331.93399999999997</v>
       </c>
-    </row>
-    <row r="13" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K12" s="2">
+        <v>30.5</v>
+      </c>
+      <c r="M12" s="3">
+        <v>43831</v>
+      </c>
+      <c r="N12" s="13">
+        <v>61.55</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>12</v>
       </c>
@@ -668,8 +819,20 @@
       <c r="H13" s="10">
         <v>346.096</v>
       </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K13" s="2">
+        <v>0.31</v>
+      </c>
+      <c r="M13" s="3">
+        <v>43862</v>
+      </c>
+      <c r="N13" s="13">
+        <v>60.48</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
@@ -688,8 +851,20 @@
       <c r="H14" s="8">
         <v>-150</v>
       </c>
-    </row>
-    <row r="15" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K14" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="M14" s="3">
+        <v>43891</v>
+      </c>
+      <c r="N14" s="13">
+        <v>58.48</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
         <v>11</v>
       </c>
@@ -708,8 +883,14 @@
       <c r="H15" s="8">
         <v>-150</v>
       </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="M15" s="3">
+        <v>43922</v>
+      </c>
+      <c r="N15" s="13">
+        <v>55.65</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="E16" s="5">
         <v>43815</v>
       </c>
@@ -722,8 +903,14 @@
       <c r="H16" s="6">
         <v>295.85000000000002</v>
       </c>
-    </row>
-    <row r="17" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M16" s="3">
+        <v>43952</v>
+      </c>
+      <c r="N16" s="13">
+        <v>54.851999999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E17" s="7">
         <v>43815</v>
       </c>
@@ -736,8 +923,14 @@
       <c r="H17" s="8">
         <v>327.666</v>
       </c>
-    </row>
-    <row r="18" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M17" s="3">
+        <v>43983</v>
+      </c>
+      <c r="N17" s="13">
+        <v>53.65</v>
+      </c>
+    </row>
+    <row r="18" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E18" s="7">
         <v>43815</v>
       </c>
@@ -750,8 +943,14 @@
       <c r="H18" s="8">
         <v>331.93399999999997</v>
       </c>
-    </row>
-    <row r="19" spans="5:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M18" s="3">
+        <v>44013</v>
+      </c>
+      <c r="N18" s="13">
+        <v>53.98</v>
+      </c>
+    </row>
+    <row r="19" spans="5:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E19" s="9">
         <v>43815</v>
       </c>
@@ -764,8 +963,14 @@
       <c r="H19" s="10">
         <v>346.096</v>
       </c>
-    </row>
-    <row r="20" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M19" s="3">
+        <v>44044</v>
+      </c>
+      <c r="N19" s="13">
+        <v>54.25</v>
+      </c>
+    </row>
+    <row r="20" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E20" s="3">
         <v>43922</v>
       </c>
@@ -778,8 +983,14 @@
       <c r="H20" s="4">
         <v>317.39999999999998</v>
       </c>
-    </row>
-    <row r="21" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M20" s="3">
+        <v>44075</v>
+      </c>
+      <c r="N20" s="13">
+        <v>56.597999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E21" s="3">
         <v>43922</v>
       </c>
@@ -792,8 +1003,14 @@
       <c r="H21" s="4">
         <v>320.8</v>
       </c>
-    </row>
-    <row r="22" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M21" s="3">
+        <v>44105</v>
+      </c>
+      <c r="N21" s="13">
+        <v>59.54</v>
+      </c>
+    </row>
+    <row r="22" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E22" s="3">
         <v>43922</v>
       </c>
@@ -806,8 +1023,14 @@
       <c r="H22" s="4">
         <v>324.8</v>
       </c>
-    </row>
-    <row r="23" spans="5:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M22" s="3">
+        <v>44136</v>
+      </c>
+      <c r="N22" s="13">
+        <v>60.65</v>
+      </c>
+    </row>
+    <row r="23" spans="5:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E23" s="3">
         <v>43922</v>
       </c>
@@ -820,8 +1043,14 @@
       <c r="H23" s="4">
         <v>331.6</v>
       </c>
-    </row>
-    <row r="24" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M23" s="3">
+        <v>44166</v>
+      </c>
+      <c r="N23" s="13">
+        <v>62.64</v>
+      </c>
+    </row>
+    <row r="24" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E24" s="5">
         <v>44024</v>
       </c>
@@ -834,8 +1063,14 @@
       <c r="H24" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="5:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M24" s="3">
+        <v>44197</v>
+      </c>
+      <c r="N24" s="13">
+        <v>63.58</v>
+      </c>
+    </row>
+    <row r="25" spans="5:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E25" s="9">
         <v>44024</v>
       </c>
@@ -848,8 +1083,14 @@
       <c r="H25" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M25" s="3">
+        <v>44228</v>
+      </c>
+      <c r="N25" s="13">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E26" s="3">
         <v>44055</v>
       </c>
@@ -862,8 +1103,14 @@
       <c r="H26" s="4">
         <v>317.39999999999998</v>
       </c>
-    </row>
-    <row r="27" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M26" s="3">
+        <v>44256</v>
+      </c>
+      <c r="N26" s="13">
+        <v>58.65</v>
+      </c>
+    </row>
+    <row r="27" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E27" s="3">
         <v>44055</v>
       </c>
@@ -876,8 +1123,14 @@
       <c r="H27" s="4">
         <v>320.8</v>
       </c>
-    </row>
-    <row r="28" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M27" s="3">
+        <v>44287</v>
+      </c>
+      <c r="N27" s="13">
+        <v>56.87</v>
+      </c>
+    </row>
+    <row r="28" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E28" s="3">
         <v>44055</v>
       </c>
@@ -890,8 +1143,10 @@
       <c r="H28" s="4">
         <v>324.8</v>
       </c>
-    </row>
-    <row r="29" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M28" s="3"/>
+      <c r="N28" s="13"/>
+    </row>
+    <row r="29" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E29" s="3">
         <v>44055</v>
       </c>
@@ -904,500 +1159,642 @@
       <c r="H29" s="4">
         <v>331.6</v>
       </c>
-    </row>
-    <row r="30" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M29" s="3"/>
+      <c r="N29" s="13"/>
+    </row>
+    <row r="30" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E30" s="3"/>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
-    </row>
-    <row r="31" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M30" s="3"/>
+      <c r="N30" s="13"/>
+    </row>
+    <row r="31" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E31" s="3"/>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
-    </row>
-    <row r="32" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M31" s="3"/>
+      <c r="N31" s="13"/>
+    </row>
+    <row r="32" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E32" s="3"/>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
-    </row>
-    <row r="33" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M32" s="3"/>
+      <c r="N32" s="13"/>
+    </row>
+    <row r="33" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E33" s="3"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
-    </row>
-    <row r="34" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M33" s="3"/>
+      <c r="N33" s="13"/>
+    </row>
+    <row r="34" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E34" s="3"/>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
-    </row>
-    <row r="35" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M34" s="3"/>
+      <c r="N34" s="13"/>
+    </row>
+    <row r="35" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E35" s="3"/>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
-    </row>
-    <row r="36" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M35" s="3"/>
+      <c r="N35" s="13"/>
+    </row>
+    <row r="36" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E36" s="3"/>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
-    </row>
-    <row r="37" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M36" s="3"/>
+      <c r="N36" s="13"/>
+    </row>
+    <row r="37" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E37" s="3"/>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
-    </row>
-    <row r="38" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M37" s="3"/>
+      <c r="N37" s="13"/>
+    </row>
+    <row r="38" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E38" s="3"/>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
-    </row>
-    <row r="39" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M38" s="3"/>
+      <c r="N38" s="13"/>
+    </row>
+    <row r="39" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E39" s="3"/>
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
       <c r="H39" s="4"/>
-    </row>
-    <row r="40" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M39" s="3"/>
+      <c r="N39" s="13"/>
+    </row>
+    <row r="40" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E40" s="3"/>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
-    </row>
-    <row r="41" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M40" s="3"/>
+      <c r="N40" s="13"/>
+    </row>
+    <row r="41" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E41" s="3"/>
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
       <c r="H41" s="4"/>
-    </row>
-    <row r="42" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M41" s="3"/>
+      <c r="N41" s="13"/>
+    </row>
+    <row r="42" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E42" s="3"/>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
       <c r="H42" s="4"/>
-    </row>
-    <row r="43" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M42" s="3"/>
+      <c r="N42" s="13"/>
+    </row>
+    <row r="43" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E43" s="3"/>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
       <c r="H43" s="4"/>
-    </row>
-    <row r="44" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M43" s="3"/>
+      <c r="N43" s="13"/>
+    </row>
+    <row r="44" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E44" s="3"/>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
-    </row>
-    <row r="45" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M44" s="3"/>
+      <c r="N44" s="13"/>
+    </row>
+    <row r="45" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E45" s="3"/>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
-    </row>
-    <row r="46" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M45" s="3"/>
+      <c r="N45" s="13"/>
+    </row>
+    <row r="46" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E46" s="3"/>
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
-    </row>
-    <row r="47" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M46" s="3"/>
+      <c r="N46" s="13"/>
+    </row>
+    <row r="47" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E47" s="3"/>
       <c r="F47" s="4"/>
       <c r="G47" s="4"/>
       <c r="H47" s="4"/>
-    </row>
-    <row r="48" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M47" s="3"/>
+      <c r="N47" s="13"/>
+    </row>
+    <row r="48" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E48" s="3"/>
       <c r="F48" s="4"/>
       <c r="G48" s="4"/>
       <c r="H48" s="4"/>
-    </row>
-    <row r="49" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M48" s="3"/>
+      <c r="N48" s="13"/>
+    </row>
+    <row r="49" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E49" s="3"/>
       <c r="F49" s="4"/>
       <c r="G49" s="4"/>
       <c r="H49" s="4"/>
-    </row>
-    <row r="50" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M49" s="3"/>
+      <c r="N49" s="13"/>
+    </row>
+    <row r="50" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E50" s="3"/>
       <c r="F50" s="4"/>
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
-    </row>
-    <row r="51" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M50" s="3"/>
+      <c r="N50" s="13"/>
+    </row>
+    <row r="51" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E51" s="3"/>
       <c r="F51" s="4"/>
       <c r="G51" s="4"/>
       <c r="H51" s="4"/>
-    </row>
-    <row r="52" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M51" s="3"/>
+      <c r="N51" s="13"/>
+    </row>
+    <row r="52" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E52" s="3"/>
       <c r="F52" s="4"/>
       <c r="G52" s="4"/>
       <c r="H52" s="4"/>
-    </row>
-    <row r="53" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M52" s="3"/>
+      <c r="N52" s="13"/>
+    </row>
+    <row r="53" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E53" s="3"/>
       <c r="F53" s="4"/>
       <c r="G53" s="4"/>
       <c r="H53" s="4"/>
-    </row>
-    <row r="54" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M53" s="3"/>
+      <c r="N53" s="13"/>
+    </row>
+    <row r="54" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E54" s="3"/>
       <c r="F54" s="4"/>
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
-    </row>
-    <row r="55" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M54" s="3"/>
+      <c r="N54" s="13"/>
+    </row>
+    <row r="55" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E55" s="3"/>
       <c r="F55" s="4"/>
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
-    </row>
-    <row r="56" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M55" s="3"/>
+      <c r="N55" s="13"/>
+    </row>
+    <row r="56" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E56" s="3"/>
       <c r="F56" s="4"/>
       <c r="G56" s="4"/>
       <c r="H56" s="4"/>
-    </row>
-    <row r="57" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M56" s="3"/>
+      <c r="N56" s="13"/>
+    </row>
+    <row r="57" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E57" s="3"/>
       <c r="F57" s="4"/>
       <c r="G57" s="4"/>
       <c r="H57" s="4"/>
-    </row>
-    <row r="58" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M57" s="3"/>
+      <c r="N57" s="13"/>
+    </row>
+    <row r="58" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E58" s="3"/>
       <c r="F58" s="4"/>
       <c r="G58" s="4"/>
       <c r="H58" s="4"/>
-    </row>
-    <row r="59" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M58" s="3"/>
+      <c r="N58" s="13"/>
+    </row>
+    <row r="59" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E59" s="3"/>
       <c r="F59" s="4"/>
       <c r="G59" s="4"/>
       <c r="H59" s="4"/>
-    </row>
-    <row r="60" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M59" s="3"/>
+      <c r="N59" s="13"/>
+    </row>
+    <row r="60" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E60" s="3"/>
       <c r="F60" s="4"/>
       <c r="G60" s="4"/>
       <c r="H60" s="4"/>
-    </row>
-    <row r="61" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M60" s="3"/>
+      <c r="N60" s="13"/>
+    </row>
+    <row r="61" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E61" s="3"/>
       <c r="F61" s="4"/>
       <c r="G61" s="4"/>
       <c r="H61" s="4"/>
-    </row>
-    <row r="62" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M61" s="3"/>
+      <c r="N61" s="13"/>
+    </row>
+    <row r="62" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E62" s="3"/>
       <c r="F62" s="4"/>
       <c r="G62" s="4"/>
       <c r="H62" s="4"/>
-    </row>
-    <row r="63" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M62" s="3"/>
+      <c r="N62" s="13"/>
+    </row>
+    <row r="63" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E63" s="3"/>
       <c r="F63" s="4"/>
       <c r="G63" s="4"/>
       <c r="H63" s="4"/>
-    </row>
-    <row r="64" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M63" s="3"/>
+      <c r="N63" s="13"/>
+    </row>
+    <row r="64" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E64" s="3"/>
       <c r="F64" s="4"/>
       <c r="G64" s="4"/>
       <c r="H64" s="4"/>
-    </row>
-    <row r="65" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M64" s="3"/>
+      <c r="N64" s="13"/>
+    </row>
+    <row r="65" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E65" s="3"/>
       <c r="F65" s="4"/>
       <c r="G65" s="4"/>
       <c r="H65" s="4"/>
-    </row>
-    <row r="66" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M65" s="3"/>
+      <c r="N65" s="13"/>
+    </row>
+    <row r="66" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E66" s="3"/>
       <c r="F66" s="4"/>
       <c r="G66" s="4"/>
       <c r="H66" s="4"/>
-    </row>
-    <row r="67" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M66" s="3"/>
+      <c r="N66" s="13"/>
+    </row>
+    <row r="67" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E67" s="3"/>
       <c r="F67" s="4"/>
       <c r="G67" s="4"/>
       <c r="H67" s="4"/>
-    </row>
-    <row r="68" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M67" s="3"/>
+      <c r="N67" s="13"/>
+    </row>
+    <row r="68" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E68" s="3"/>
       <c r="F68" s="4"/>
       <c r="G68" s="4"/>
       <c r="H68" s="4"/>
-    </row>
-    <row r="69" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M68" s="3"/>
+      <c r="N68" s="13"/>
+    </row>
+    <row r="69" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E69" s="3"/>
       <c r="F69" s="4"/>
       <c r="G69" s="4"/>
       <c r="H69" s="4"/>
-    </row>
-    <row r="70" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M69" s="3"/>
+      <c r="N69" s="13"/>
+    </row>
+    <row r="70" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E70" s="3"/>
       <c r="F70" s="4"/>
       <c r="G70" s="4"/>
       <c r="H70" s="4"/>
-    </row>
-    <row r="71" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M70" s="3"/>
+      <c r="N70" s="13"/>
+    </row>
+    <row r="71" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E71" s="3"/>
       <c r="F71" s="4"/>
       <c r="G71" s="4"/>
       <c r="H71" s="4"/>
-    </row>
-    <row r="72" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M71" s="3"/>
+      <c r="N71" s="13"/>
+    </row>
+    <row r="72" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E72" s="3"/>
       <c r="F72" s="4"/>
       <c r="G72" s="4"/>
       <c r="H72" s="4"/>
-    </row>
-    <row r="73" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M72" s="3"/>
+      <c r="N72" s="13"/>
+    </row>
+    <row r="73" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E73" s="3"/>
       <c r="F73" s="4"/>
       <c r="G73" s="4"/>
       <c r="H73" s="4"/>
-    </row>
-    <row r="74" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M73" s="3"/>
+      <c r="N73" s="13"/>
+    </row>
+    <row r="74" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E74" s="3"/>
       <c r="F74" s="4"/>
       <c r="G74" s="4"/>
       <c r="H74" s="4"/>
-    </row>
-    <row r="75" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M74" s="3"/>
+      <c r="N74" s="13"/>
+    </row>
+    <row r="75" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E75" s="3"/>
       <c r="F75" s="4"/>
       <c r="G75" s="4"/>
       <c r="H75" s="4"/>
-    </row>
-    <row r="76" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M75" s="3"/>
+      <c r="N75" s="13"/>
+    </row>
+    <row r="76" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E76" s="3"/>
       <c r="F76" s="4"/>
       <c r="G76" s="4"/>
       <c r="H76" s="4"/>
-    </row>
-    <row r="77" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M76" s="3"/>
+      <c r="N76" s="13"/>
+    </row>
+    <row r="77" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E77" s="3"/>
       <c r="F77" s="4"/>
       <c r="G77" s="4"/>
       <c r="H77" s="4"/>
-    </row>
-    <row r="78" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M77" s="3"/>
+      <c r="N77" s="13"/>
+    </row>
+    <row r="78" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E78" s="3"/>
       <c r="F78" s="4"/>
       <c r="G78" s="4"/>
       <c r="H78" s="4"/>
-    </row>
-    <row r="79" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M78" s="3"/>
+      <c r="N78" s="13"/>
+    </row>
+    <row r="79" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E79" s="3"/>
       <c r="F79" s="4"/>
       <c r="G79" s="4"/>
       <c r="H79" s="4"/>
-    </row>
-    <row r="80" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M79" s="3"/>
+      <c r="N79" s="13"/>
+    </row>
+    <row r="80" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E80" s="3"/>
       <c r="F80" s="4"/>
       <c r="G80" s="4"/>
       <c r="H80" s="4"/>
-    </row>
-    <row r="81" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M80" s="3"/>
+      <c r="N80" s="13"/>
+    </row>
+    <row r="81" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E81" s="3"/>
       <c r="F81" s="4"/>
       <c r="G81" s="4"/>
       <c r="H81" s="4"/>
-    </row>
-    <row r="82" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M81" s="3"/>
+      <c r="N81" s="13"/>
+    </row>
+    <row r="82" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E82" s="3"/>
       <c r="F82" s="4"/>
       <c r="G82" s="4"/>
       <c r="H82" s="4"/>
-    </row>
-    <row r="83" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M82" s="3"/>
+      <c r="N82" s="13"/>
+    </row>
+    <row r="83" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E83" s="3"/>
       <c r="F83" s="4"/>
       <c r="G83" s="4"/>
       <c r="H83" s="4"/>
-    </row>
-    <row r="84" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M83" s="3"/>
+      <c r="N83" s="13"/>
+    </row>
+    <row r="84" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E84" s="3"/>
       <c r="F84" s="4"/>
       <c r="G84" s="4"/>
       <c r="H84" s="4"/>
-    </row>
-    <row r="85" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M84" s="3"/>
+      <c r="N84" s="13"/>
+    </row>
+    <row r="85" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E85" s="3"/>
       <c r="F85" s="4"/>
       <c r="G85" s="4"/>
       <c r="H85" s="4"/>
-    </row>
-    <row r="86" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M85" s="3"/>
+      <c r="N85" s="13"/>
+    </row>
+    <row r="86" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E86" s="3"/>
       <c r="F86" s="4"/>
       <c r="G86" s="4"/>
       <c r="H86" s="4"/>
-    </row>
-    <row r="87" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M86" s="3"/>
+      <c r="N86" s="13"/>
+    </row>
+    <row r="87" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E87" s="3"/>
       <c r="F87" s="4"/>
       <c r="G87" s="4"/>
       <c r="H87" s="4"/>
-    </row>
-    <row r="88" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M87" s="3"/>
+      <c r="N87" s="13"/>
+    </row>
+    <row r="88" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E88" s="3"/>
       <c r="F88" s="4"/>
       <c r="G88" s="4"/>
       <c r="H88" s="4"/>
-    </row>
-    <row r="89" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M88" s="3"/>
+      <c r="N88" s="13"/>
+    </row>
+    <row r="89" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E89" s="3"/>
       <c r="F89" s="4"/>
       <c r="G89" s="4"/>
       <c r="H89" s="4"/>
-    </row>
-    <row r="90" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M89" s="3"/>
+      <c r="N89" s="13"/>
+    </row>
+    <row r="90" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E90" s="3"/>
       <c r="F90" s="4"/>
       <c r="G90" s="4"/>
       <c r="H90" s="4"/>
-    </row>
-    <row r="91" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M90" s="3"/>
+      <c r="N90" s="13"/>
+    </row>
+    <row r="91" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E91" s="3"/>
       <c r="F91" s="4"/>
       <c r="G91" s="4"/>
       <c r="H91" s="4"/>
-    </row>
-    <row r="92" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M91" s="3"/>
+      <c r="N91" s="13"/>
+    </row>
+    <row r="92" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E92" s="3"/>
       <c r="F92" s="4"/>
       <c r="G92" s="4"/>
       <c r="H92" s="4"/>
-    </row>
-    <row r="93" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M92" s="3"/>
+      <c r="N92" s="13"/>
+    </row>
+    <row r="93" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E93" s="3"/>
       <c r="F93" s="4"/>
       <c r="G93" s="4"/>
       <c r="H93" s="4"/>
-    </row>
-    <row r="94" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M93" s="3"/>
+      <c r="N93" s="13"/>
+    </row>
+    <row r="94" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E94" s="3"/>
       <c r="F94" s="4"/>
       <c r="G94" s="4"/>
       <c r="H94" s="4"/>
-    </row>
-    <row r="95" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M94" s="3"/>
+      <c r="N94" s="13"/>
+    </row>
+    <row r="95" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E95" s="3"/>
       <c r="F95" s="4"/>
       <c r="G95" s="4"/>
       <c r="H95" s="4"/>
-    </row>
-    <row r="96" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M95" s="3"/>
+      <c r="N95" s="13"/>
+    </row>
+    <row r="96" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E96" s="3"/>
       <c r="F96" s="4"/>
       <c r="G96" s="4"/>
       <c r="H96" s="4"/>
-    </row>
-    <row r="97" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M96" s="3"/>
+      <c r="N96" s="13"/>
+    </row>
+    <row r="97" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E97" s="3"/>
       <c r="F97" s="4"/>
       <c r="G97" s="4"/>
       <c r="H97" s="4"/>
-    </row>
-    <row r="98" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M97" s="3"/>
+      <c r="N97" s="13"/>
+    </row>
+    <row r="98" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E98" s="3"/>
       <c r="F98" s="4"/>
       <c r="G98" s="4"/>
       <c r="H98" s="4"/>
-    </row>
-    <row r="99" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M98" s="3"/>
+      <c r="N98" s="13"/>
+    </row>
+    <row r="99" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E99" s="3"/>
       <c r="F99" s="4"/>
       <c r="G99" s="4"/>
       <c r="H99" s="4"/>
-    </row>
-    <row r="100" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="M99" s="3"/>
+      <c r="N99" s="13"/>
+    </row>
+    <row r="100" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E100" s="3"/>
       <c r="F100" s="4"/>
       <c r="G100" s="4"/>
       <c r="H100" s="4"/>
     </row>
-    <row r="101" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E101" s="3"/>
       <c r="F101" s="4"/>
       <c r="G101" s="4"/>
       <c r="H101" s="4"/>
     </row>
-    <row r="102" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E102" s="3"/>
       <c r="F102" s="4"/>
       <c r="G102" s="4"/>
       <c r="H102" s="4"/>
     </row>
-    <row r="103" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E103" s="3"/>
       <c r="F103" s="4"/>
       <c r="G103" s="4"/>
       <c r="H103" s="4"/>
     </row>
-    <row r="104" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E104" s="3"/>
       <c r="F104" s="4"/>
       <c r="G104" s="4"/>
       <c r="H104" s="4"/>
     </row>
-    <row r="105" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E105" s="3"/>
       <c r="F105" s="4"/>
       <c r="G105" s="4"/>
       <c r="H105" s="4"/>
     </row>
-    <row r="106" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E106" s="3"/>
       <c r="F106" s="4"/>
       <c r="G106" s="4"/>
       <c r="H106" s="4"/>
     </row>
-    <row r="107" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E107" s="3"/>
       <c r="F107" s="4"/>
       <c r="G107" s="4"/>
       <c r="H107" s="4"/>
     </row>
-    <row r="108" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E108" s="3"/>
       <c r="F108" s="4"/>
       <c r="G108" s="4"/>
       <c r="H108" s="4"/>
     </row>
-    <row r="109" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E109" s="3"/>
       <c r="F109" s="4"/>
       <c r="G109" s="4"/>
       <c r="H109" s="4"/>
     </row>
-    <row r="110" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E110" s="3"/>
       <c r="F110" s="4"/>
       <c r="G110" s="4"/>
       <c r="H110" s="4"/>
     </row>
-    <row r="111" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E111" s="3"/>
       <c r="F111" s="4"/>
       <c r="G111" s="4"/>
       <c r="H111" s="4"/>
     </row>
-    <row r="112" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E112" s="3"/>
       <c r="F112" s="4"/>
       <c r="G112" s="4"/>
@@ -2478,6 +2875,78 @@
       <c r="H291" s="4"/>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K8" xr:uid="{851CFE34-DBF7-4E8E-8342-553973F79B04}">
+      <formula1>"TRUE,FALSE"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{721564D4-5F2D-4B24-ADC0-DEA0F505F4CA}">
+  <dimension ref="B2:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
First cut at getting properties of calclation results.
</commit_message>
<xml_diff>
--- a/samples/excel/three_factor_storage.xlsx
+++ b/samples/excel/three_factor_storage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jake\source\repos\storage\samples\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{057B534F-60E9-487C-B9B3-135D3ED38A32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55AD7FFD-9FFA-4EDE-A440-F12C02C9BC11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
   <si>
     <t>Inject/Withdraw/Inventory Constraints</t>
   </si>
@@ -176,13 +176,16 @@
     <t>Rate</t>
   </si>
   <si>
-    <t>3-factor val1</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
     <t>Progress</t>
+  </si>
+  <si>
+    <t>3-factor val4</t>
+  </si>
+  <si>
+    <t>NPV</t>
   </si>
 </sst>
 </file>
@@ -273,7 +276,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -293,6 +296,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -310,6 +314,21 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
+<volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <volType type="realTimeData">
+    <main first="rtdsrv.94072a11ef8c4c3b924035f0383dfad0">
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>3c477e86-36fe-4954-88ab-a8d157dd996f</stp>
+        <tr r="W10" s="1"/>
+      </tp>
+    </main>
+  </volType>
+</volTypes>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -577,8 +596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:W2391"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W16" sqref="W16"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="W11" sqref="W11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,6 +611,8 @@
     <col min="16" max="16" width="10.85546875" customWidth="1"/>
     <col min="19" max="19" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="11.85546875" customWidth="1"/>
+    <col min="23" max="23" width="12" customWidth="1"/>
+    <col min="24" max="24" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:23" x14ac:dyDescent="0.25">
@@ -703,11 +724,11 @@
         <v>50.640695748227039</v>
       </c>
       <c r="V6" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="W6" s="16" t="str" cm="1">
         <f t="array" ref="W6">_xll.cmdty.StorageValueThreeFactor(V6, C2, K6,K7,S6:T2391, M6:N99,K11,K12,K13,K14,K8,'Static Data'!B4:C145, McParams.NumSims, McParams.BasisFuncs, McParams.Seed, McParams.FwdSeed, McParams.GridPoints, McParams.NumTol, McParams.ExtraDecs)</f>
-        <v>3-factor val1</v>
+        <v>3-factor val4</v>
       </c>
     </row>
     <row r="7" spans="2:23" x14ac:dyDescent="0.25">
@@ -756,7 +777,7 @@
         <v>49.700092287036142</v>
       </c>
       <c r="V7" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="W7" t="str" cm="1">
         <f t="array" ref="W7">_xll.cmdty.SubscribeStatus(W6)</f>
@@ -803,7 +824,7 @@
         <v>49.700092287036142</v>
       </c>
       <c r="V8" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="W8" s="18" cm="1">
         <f t="array" ref="W8">_xll.cmdty.SubscribeProgress(W6)</f>
@@ -888,6 +909,13 @@
       <c r="T10" s="12">
         <f t="shared" si="1"/>
         <v>49.700092287036142</v>
+      </c>
+      <c r="V10" t="s">
+        <v>39</v>
+      </c>
+      <c r="W10" s="19" cm="1">
+        <f t="array" ref="W10">_xll.cmdty.SubscribeResultProperty(W6,V10, NA())</f>
+        <v>415419.8808551383</v>
       </c>
     </row>
     <row r="11" spans="2:23" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added progress bar chart formatting.
</commit_message>
<xml_diff>
--- a/samples/excel/three_factor_storage.xlsx
+++ b/samples/excel/three_factor_storage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jake\source\repos\storage\samples\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55AD7FFD-9FFA-4EDE-A440-F12C02C9BC11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5D95456-2DFE-4642-AF15-AB8B168A6E6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -182,10 +182,10 @@
     <t>Progress</t>
   </si>
   <si>
-    <t>3-factor val4</t>
+    <t>NPV</t>
   </si>
   <si>
-    <t>NPV</t>
+    <t>3-factor val5</t>
   </si>
 </sst>
 </file>
@@ -276,7 +276,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -295,8 +295,11 @@
     <xf numFmtId="15" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -314,21 +317,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
-<volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <volType type="realTimeData">
-    <main first="rtdsrv.94072a11ef8c4c3b924035f0383dfad0">
-      <tp>
-        <v>1</v>
-        <stp/>
-        <stp>3c477e86-36fe-4954-88ab-a8d157dd996f</stp>
-        <tr r="W10" s="1"/>
-      </tp>
-    </main>
-  </volType>
-</volTypes>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -597,7 +585,7 @@
   <dimension ref="B2:W2391"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W11" sqref="W11"/>
+      <selection activeCell="Y8" sqref="Y8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,7 +599,7 @@
     <col min="16" max="16" width="10.85546875" customWidth="1"/>
     <col min="19" max="19" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="11.85546875" customWidth="1"/>
-    <col min="23" max="23" width="12" customWidth="1"/>
+    <col min="23" max="23" width="14.85546875" customWidth="1"/>
     <col min="24" max="24" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -724,11 +712,11 @@
         <v>50.640695748227039</v>
       </c>
       <c r="V6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="W6" s="16" t="str" cm="1">
         <f t="array" ref="W6">_xll.cmdty.StorageValueThreeFactor(V6, C2, K6,K7,S6:T2391, M6:N99,K11,K12,K13,K14,K8,'Static Data'!B4:C145, McParams.NumSims, McParams.BasisFuncs, McParams.Seed, McParams.FwdSeed, McParams.GridPoints, McParams.NumTol, McParams.ExtraDecs)</f>
-        <v>3-factor val4</v>
+        <v>3-factor val5</v>
       </c>
     </row>
     <row r="7" spans="2:23" x14ac:dyDescent="0.25">
@@ -781,7 +769,7 @@
       </c>
       <c r="W7" t="str" cm="1">
         <f t="array" ref="W7">_xll.cmdty.SubscribeStatus(W6)</f>
-        <v>Running</v>
+        <v>Success</v>
       </c>
     </row>
     <row r="8" spans="2:23" x14ac:dyDescent="0.25">
@@ -826,7 +814,7 @@
       <c r="V8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="W8" s="18" cm="1">
+      <c r="W8" s="19" cm="1">
         <f t="array" ref="W8">_xll.cmdty.SubscribeProgress(W6)</f>
         <v>1</v>
       </c>
@@ -911,11 +899,11 @@
         <v>49.700092287036142</v>
       </c>
       <c r="V10" t="s">
-        <v>39</v>
-      </c>
-      <c r="W10" s="19" cm="1">
+        <v>38</v>
+      </c>
+      <c r="W10" s="18" cm="1">
         <f t="array" ref="W10">_xll.cmdty.SubscribeResultProperty(W6,V10, NA())</f>
-        <v>415419.8808551383</v>
+        <v>424782.1137813027</v>
       </c>
     </row>
     <row r="11" spans="2:23" x14ac:dyDescent="0.25">
@@ -26482,6 +26470,20 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="W8">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{F1287CA2-4C5F-4092-B7AF-37CD946CD0A1}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K8" xr:uid="{851CFE34-DBF7-4E8E-8342-553973F79B04}">
       <formula1>"TRUE,FALSE"</formula1>
@@ -26489,6 +26491,27 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{F1287CA2-4C5F-4092-B7AF-37CD946CD0A1}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>W8</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -26497,7 +26520,7 @@
   <dimension ref="B2:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26509,8 +26532,8 @@
       <c r="B2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="2">
-        <v>1000</v>
+      <c r="C2" s="20">
+        <v>5000</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
@@ -26563,9 +26586,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{606CC08C-FC66-446C-A778-C16CE1C2D79E}">
   <dimension ref="B2:C110"/>
   <sheetViews>
-    <sheetView topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>